<commit_message>
Updates toward finalizing for publication
smaller errors, bigger errors, removing references to multicommodity systems
</commit_message>
<xml_diff>
--- a/input_files/user_defined/Scenario setup.xlsx
+++ b/input_files/user_defined/Scenario setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/input_files/user_defined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0073A8-6AC0-A24B-86EC-0001EF615DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA0098-7DDC-AA4D-A7F4-A72C07EE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="12040" windowHeight="16080" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="335">
   <si>
     <t>Parameter category</t>
   </si>
@@ -972,13 +972,82 @@
   </si>
   <si>
     <t>Disclaimer on fabrication efficiency and lifetime mean and standard deviation: we do not currently have it setup to dynamically change this value - changing it in 2003 would change how much scrap reaches end of life in 2003, as the lifetimes go into the cumulative density function determining this value directly, rather than setting the lifetime of products going forward. To get the desired effect, you would likely have to use a year farther in the future for the sector you are considering. This model is not stock driven, so changing lifetimes and fabrication efficiencies also will not change demand trajectories aside from the impacts the change in scrap generation has on prices and therefore demand. Fabrication efficiency changes will only impact the quantity of new scrap generated.</t>
+  </si>
+  <si>
+    <t>Scenario 6</t>
+  </si>
+  <si>
+    <t>Percent increase in scrap supply per year after the initial total percent change ramp finishes. If using this, need to have a value set for the total increase in scrap supply variable, otherwise all will be zero.</t>
+  </si>
+  <si>
+    <t>Scenario 7</t>
+  </si>
+  <si>
+    <t>Scenario 8</t>
+  </si>
+  <si>
+    <t>Scenario 9</t>
+  </si>
+  <si>
+    <t>Scenario 10</t>
+  </si>
+  <si>
+    <t>Scenario 11</t>
+  </si>
+  <si>
+    <t>Scenario 12</t>
+  </si>
+  <si>
+    <t>Scenario 13</t>
+  </si>
+  <si>
+    <t>Year 4</t>
+  </si>
+  <si>
+    <t>Year 5</t>
+  </si>
+  <si>
+    <t>Year 6</t>
+  </si>
+  <si>
+    <t>Year 7</t>
+  </si>
+  <si>
+    <t>Year 8</t>
+  </si>
+  <si>
+    <t>Year 9</t>
+  </si>
+  <si>
+    <t>Year 10</t>
+  </si>
+  <si>
+    <t>Year 11</t>
+  </si>
+  <si>
+    <t>Year 12</t>
+  </si>
+  <si>
+    <t>Year 13</t>
+  </si>
+  <si>
+    <t>Year 14</t>
+  </si>
+  <si>
+    <t>Year 15</t>
+  </si>
+  <si>
+    <t>Year 16</t>
+  </si>
+  <si>
+    <t>Year 17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1021,6 +1090,12 @@
       <b/>
       <sz val="12"/>
       <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1071,7 +1146,151 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1094,22 +1313,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:M96" totalsRowShown="0">
-  <autoFilter ref="A1:M96" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:AI96" totalsRowShown="0">
+  <autoFilter ref="A1:AI96" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}"/>
+  <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{C4332FCF-8E4C-4F49-8EFC-804C6E3A59B2}" name="Parameter category"/>
-    <tableColumn id="2" xr3:uid="{A55A75DB-88A1-1245-BF1A-68A78F78C819}" name="Parameter name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A55A75DB-88A1-1245-BF1A-68A78F78C819}" name="Parameter name" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{5A41921B-736C-6B44-9ECB-CB018A2EAD98}" name="Variable name"/>
     <tableColumn id="4" xr3:uid="{AC20CA22-09A0-874C-8AAB-D90343AC4C41}" name="Description"/>
-    <tableColumn id="5" xr3:uid="{BC697E1E-B29C-C449-B77E-41BE3FCCCC5F}" name="Tuning range or preset value" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{BC697E1E-B29C-C449-B77E-41BE3FCCCC5F}" name="Tuning range or preset value" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{5E98ED95-4E7B-3B45-A47B-AF1FEE1A9A80}" name="Scenario 1"/>
     <tableColumn id="7" xr3:uid="{D0B2B3FA-F3D8-C746-B783-084B2C487DBB}" name="Scenario 2"/>
     <tableColumn id="8" xr3:uid="{BB62F53F-FC7E-0241-8EFE-9D0D4B695FC4}" name="Scenario 3"/>
     <tableColumn id="9" xr3:uid="{71A5D20F-2653-0746-B54E-2208868C584B}" name="Scenario 4"/>
     <tableColumn id="10" xr3:uid="{57545BB2-994C-E14B-995E-1E22F5BA7322}" name="Scenario 5"/>
+    <tableColumn id="22" xr3:uid="{6902B9B4-8E0D-2646-885E-EDD1EE6854F9}" name="Scenario 6" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{0219D9D3-A7AF-B649-9720-C5C56B6DA494}" name="Scenario 7" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{C0DF87A7-EA0E-5549-9DAF-C7D237CAC211}" name="Scenario 8" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{1003B7E9-86E5-BD44-8CF1-08E412F43519}" name="Scenario 9" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{EE68D8F1-C9A3-844D-B61C-BFC4D6C540B4}" name="Scenario 10" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{AF7F194F-8762-1F4B-829B-D2951D37AEDF}" name="Scenario 11" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{CE4B6D99-C26D-3B42-90BF-E046DE5C8035}" name="Scenario 12" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{AB5BD98B-FAF8-304C-9752-E581F8FDFE2E}" name="Scenario 13" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{9EC9A262-BA04-314B-8E87-E93596D98225}" name="Year 1"/>
     <tableColumn id="12" xr3:uid="{3B932622-32D8-EB4D-B8D6-252827BECB68}" name="Year 2"/>
     <tableColumn id="13" xr3:uid="{67C9335A-4404-0B4E-A4E3-F38FEB4535CA}" name="Year 3"/>
+    <tableColumn id="23" xr3:uid="{494E6D6B-0F32-AC49-8741-B248F808E4F5}" name="Year 4"/>
+    <tableColumn id="24" xr3:uid="{CA22B1B2-1B83-D14C-BCF9-3F94A89578FD}" name="Year 5"/>
+    <tableColumn id="25" xr3:uid="{B742B88A-44C0-9C47-9E3C-4411F15854BA}" name="Year 6"/>
+    <tableColumn id="26" xr3:uid="{D60CFDE2-5FE3-9B45-970A-E505CC760C5B}" name="Year 7"/>
+    <tableColumn id="27" xr3:uid="{D7E3F1E5-8ED9-A642-BBFB-19A7B3A6C44F}" name="Year 8"/>
+    <tableColumn id="28" xr3:uid="{2380CACE-3EDB-BD46-A4CA-7271F22107BF}" name="Year 9"/>
+    <tableColumn id="29" xr3:uid="{1D2A06EA-52DD-0047-A07C-4C0E1249494F}" name="Year 10"/>
+    <tableColumn id="30" xr3:uid="{20A8D89A-738C-A145-B0C0-D614F78D35B5}" name="Year 11"/>
+    <tableColumn id="31" xr3:uid="{EA384FC8-180E-6147-A26A-0726CEB96D8D}" name="Year 12"/>
+    <tableColumn id="32" xr3:uid="{CC933E1E-2947-9140-A208-7D67D9F4ED7D}" name="Year 13"/>
+    <tableColumn id="33" xr3:uid="{6DF82DC0-3AB5-7E41-8260-F5D45989229F}" name="Year 14"/>
+    <tableColumn id="34" xr3:uid="{2DF18580-FF7F-A349-A34B-75AB6D285E5D}" name="Year 15"/>
+    <tableColumn id="35" xr3:uid="{21FFBCB7-19E6-5A4F-AE90-7F4A2F057A35}" name="Year 16"/>
+    <tableColumn id="36" xr3:uid="{75F8A80A-46DB-F74D-A07E-5BF848776206}" name="Year 17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1412,11 +1653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70A1D66-ACB3-5F43-8146-4761D363CB09}">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:AI96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,11 +1667,10 @@
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="89.5" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="10" width="13.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="18" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1462,16 +1702,82 @@
         <v>279</v>
       </c>
       <c r="K1" t="s">
+        <v>312</v>
+      </c>
+      <c r="L1" t="s">
+        <v>314</v>
+      </c>
+      <c r="M1" t="s">
+        <v>315</v>
+      </c>
+      <c r="N1" t="s">
+        <v>316</v>
+      </c>
+      <c r="O1" t="s">
+        <v>317</v>
+      </c>
+      <c r="P1" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>319</v>
+      </c>
+      <c r="R1" t="s">
+        <v>320</v>
+      </c>
+      <c r="S1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="U1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="V1" t="s">
+        <v>321</v>
+      </c>
+      <c r="W1" t="s">
+        <v>322</v>
+      </c>
+      <c r="X1" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -1488,7 +1794,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1505,7 +1811,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1522,7 +1828,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1539,7 +1845,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -1556,7 +1862,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -1573,7 +1879,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -1590,7 +1896,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -1607,7 +1913,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -1624,7 +1930,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -1641,7 +1947,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -1658,7 +1964,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -1675,7 +1981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1692,7 +1998,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -1709,7 +2015,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -1725,14 +2031,8 @@
       <c r="E16" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F16">
-        <v>0.02</v>
-      </c>
-      <c r="K16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -1748,14 +2048,8 @@
       <c r="E17" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="F17">
-        <v>0.03</v>
-      </c>
-      <c r="K17">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1772,7 +2066,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1789,7 +2083,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -1806,7 +2100,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -1823,7 +2117,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>116</v>
       </c>
@@ -1840,7 +2134,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -1857,7 +2151,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -1874,7 +2168,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -1891,7 +2185,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -1908,7 +2202,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>116</v>
       </c>
@@ -1925,7 +2219,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>196</v>
       </c>
@@ -1942,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -1959,7 +2253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>196</v>
       </c>
@@ -1976,7 +2270,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -1993,7 +2287,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>196</v>
       </c>
@@ -2282,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>196</v>
       </c>
@@ -2299,7 +2593,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>254</v>
       </c>
@@ -2315,8 +2609,68 @@
       <c r="E50" s="6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" t="b">
+        <v>0</v>
+      </c>
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+      <c r="N50" t="b">
+        <v>0</v>
+      </c>
+      <c r="O50" t="b">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>2020</v>
+      </c>
+      <c r="T50">
+        <v>2020</v>
+      </c>
+      <c r="U50">
+        <v>2020</v>
+      </c>
+      <c r="V50">
+        <v>2020</v>
+      </c>
+      <c r="W50">
+        <v>2020</v>
+      </c>
+      <c r="X50">
+        <v>2020</v>
+      </c>
+      <c r="Y50">
+        <v>2020</v>
+      </c>
+      <c r="Z50">
+        <v>2020</v>
+      </c>
+      <c r="AA50">
+        <v>2020</v>
+      </c>
+      <c r="AB50">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>254</v>
       </c>
@@ -2333,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -2349,8 +2703,68 @@
       <c r="E52" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F52">
+        <v>1</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="S52">
+        <v>2020</v>
+      </c>
+      <c r="T52">
+        <v>2020</v>
+      </c>
+      <c r="U52">
+        <v>2020</v>
+      </c>
+      <c r="V52">
+        <v>2020</v>
+      </c>
+      <c r="W52">
+        <v>2020</v>
+      </c>
+      <c r="X52">
+        <v>2020</v>
+      </c>
+      <c r="Y52">
+        <v>2020</v>
+      </c>
+      <c r="Z52">
+        <v>2020</v>
+      </c>
+      <c r="AA52">
+        <v>2020</v>
+      </c>
+      <c r="AB52">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>254</v>
       </c>
@@ -2366,8 +2780,65 @@
       <c r="E53" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>0.01</v>
+      </c>
+      <c r="H53">
+        <v>0.1</v>
+      </c>
+      <c r="I53">
+        <v>0.2</v>
+      </c>
+      <c r="J53">
+        <v>0.4</v>
+      </c>
+      <c r="K53">
+        <v>0.6</v>
+      </c>
+      <c r="L53">
+        <v>0.8</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1.5</v>
+      </c>
+      <c r="O53">
+        <v>2</v>
+      </c>
+      <c r="S53">
+        <v>2020</v>
+      </c>
+      <c r="T53">
+        <v>2020</v>
+      </c>
+      <c r="U53">
+        <v>2020</v>
+      </c>
+      <c r="V53">
+        <v>2020</v>
+      </c>
+      <c r="W53">
+        <v>2020</v>
+      </c>
+      <c r="X53">
+        <v>2020</v>
+      </c>
+      <c r="Y53">
+        <v>2020</v>
+      </c>
+      <c r="Z53">
+        <v>2020</v>
+      </c>
+      <c r="AA53">
+        <v>2020</v>
+      </c>
+      <c r="AB53">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>254</v>
       </c>
@@ -2377,11 +2848,71 @@
       <c r="C54" t="s">
         <v>257</v>
       </c>
+      <c r="D54" t="s">
+        <v>313</v>
+      </c>
       <c r="E54" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>0.01</v>
+      </c>
+      <c r="H54">
+        <v>0.1</v>
+      </c>
+      <c r="I54">
+        <v>0.2</v>
+      </c>
+      <c r="J54">
+        <v>0.4</v>
+      </c>
+      <c r="K54">
+        <v>0.6</v>
+      </c>
+      <c r="L54">
+        <v>0.8</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1.5</v>
+      </c>
+      <c r="O54">
+        <v>2</v>
+      </c>
+      <c r="S54">
+        <v>2020</v>
+      </c>
+      <c r="T54">
+        <v>2020</v>
+      </c>
+      <c r="U54">
+        <v>2020</v>
+      </c>
+      <c r="V54">
+        <v>2020</v>
+      </c>
+      <c r="W54">
+        <v>2020</v>
+      </c>
+      <c r="X54">
+        <v>2020</v>
+      </c>
+      <c r="Y54">
+        <v>2020</v>
+      </c>
+      <c r="Z54">
+        <v>2020</v>
+      </c>
+      <c r="AA54">
+        <v>2020</v>
+      </c>
+      <c r="AB54">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>254</v>
       </c>
@@ -2395,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -2409,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>254</v>
       </c>
@@ -2423,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2447,8 +2978,16 @@
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>7</v>
       </c>
@@ -2469,17 +3008,25 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
-      <c r="K59" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L59" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M59" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T59" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U59" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>7</v>
       </c>
@@ -2500,17 +3047,25 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
-      <c r="K60" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L60" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M60" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T60" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U60" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>7</v>
       </c>
@@ -2531,17 +3086,25 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-      <c r="K61" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L61" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M61" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
+      <c r="P61" s="7"/>
+      <c r="Q61" s="7"/>
+      <c r="R61" s="7"/>
+      <c r="S61" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T61" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U61" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>7</v>
       </c>
@@ -2562,17 +3125,25 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
-      <c r="K62" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L62" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M62" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T62" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U62" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>7</v>
       </c>
@@ -2593,17 +3164,25 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
-      <c r="K63" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L63" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M63" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T63" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U63" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>7</v>
       </c>
@@ -2624,17 +3203,25 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
-      <c r="K64" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L64" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M64" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T64" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U64" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>7</v>
       </c>
@@ -2655,17 +3242,25 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-      <c r="K65" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L65" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M65" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T65" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U65" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>7</v>
       </c>
@@ -2686,17 +3281,25 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
-      <c r="K66" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L66" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M66" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K66" s="7"/>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T66" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U66" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>7</v>
       </c>
@@ -2717,17 +3320,25 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-      <c r="K67" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L67" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M67" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="7"/>
+      <c r="S67" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T67" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U67" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>7</v>
       </c>
@@ -2748,17 +3359,25 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
-      <c r="K68" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L68" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M68" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T68" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U68" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>7</v>
       </c>
@@ -2779,17 +3398,25 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
-      <c r="K69" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L69" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M69" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="7"/>
+      <c r="P69" s="7"/>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7"/>
+      <c r="S69" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T69" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U69" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>7</v>
       </c>
@@ -2810,17 +3437,25 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
-      <c r="K70" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L70" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M70" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="7"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="7"/>
+      <c r="R70" s="7"/>
+      <c r="S70" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T70" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U70" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>7</v>
       </c>
@@ -2841,17 +3476,25 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
-      <c r="K71" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L71" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M71" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T71" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U71" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>7</v>
       </c>
@@ -2872,17 +3515,25 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
-      <c r="K72" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L72" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M72" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T72" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U72" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
         <v>7</v>
       </c>
@@ -2903,17 +3554,25 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-      <c r="K73" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L73" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M73" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K73" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
+      <c r="N73" s="7"/>
+      <c r="O73" s="7"/>
+      <c r="P73" s="7"/>
+      <c r="Q73" s="7"/>
+      <c r="R73" s="7"/>
+      <c r="S73" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T73" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U73" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
         <v>7</v>
       </c>
@@ -2934,17 +3593,25 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
-      <c r="K74" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L74" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M74" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K74" s="7"/>
+      <c r="L74" s="7"/>
+      <c r="M74" s="7"/>
+      <c r="N74" s="7"/>
+      <c r="O74" s="7"/>
+      <c r="P74" s="7"/>
+      <c r="Q74" s="7"/>
+      <c r="R74" s="7"/>
+      <c r="S74" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T74" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U74" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
         <v>7</v>
       </c>
@@ -2965,17 +3632,25 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-      <c r="K75" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L75" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M75" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K75" s="7"/>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7"/>
+      <c r="S75" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T75" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U75" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
         <v>7</v>
       </c>
@@ -2996,17 +3671,25 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
-      <c r="K76" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L76" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M76" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K76" s="7"/>
+      <c r="L76" s="7"/>
+      <c r="M76" s="7"/>
+      <c r="N76" s="7"/>
+      <c r="O76" s="7"/>
+      <c r="P76" s="7"/>
+      <c r="Q76" s="7"/>
+      <c r="R76" s="7"/>
+      <c r="S76" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T76" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U76" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>7</v>
       </c>
@@ -3027,17 +3710,25 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-      <c r="K77" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L77" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M77" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K77" s="7"/>
+      <c r="L77" s="7"/>
+      <c r="M77" s="7"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="7"/>
+      <c r="P77" s="7"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="7"/>
+      <c r="S77" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T77" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U77" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>7</v>
       </c>
@@ -3058,17 +3749,25 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
-      <c r="K78" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L78" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M78" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K78" s="7"/>
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T78" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U78" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>7</v>
       </c>
@@ -3089,17 +3788,25 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-      <c r="K79" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L79" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M79" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="7"/>
+      <c r="P79" s="7"/>
+      <c r="Q79" s="7"/>
+      <c r="R79" s="7"/>
+      <c r="S79" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T79" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U79" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>7</v>
       </c>
@@ -3120,17 +3827,25 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
-      <c r="K80" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L80" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M80" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="7"/>
+      <c r="O80" s="7"/>
+      <c r="P80" s="7"/>
+      <c r="Q80" s="7"/>
+      <c r="R80" s="7"/>
+      <c r="S80" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T80" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U80" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>7</v>
       </c>
@@ -3151,17 +3866,25 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
-      <c r="K81" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L81" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M81" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T81" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U81" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
         <v>7</v>
       </c>
@@ -3182,17 +3905,25 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
-      <c r="K82" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L82" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M82" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7"/>
+      <c r="O82" s="7"/>
+      <c r="P82" s="7"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T82" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U82" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
         <v>7</v>
       </c>
@@ -3213,17 +3944,25 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
-      <c r="K83" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L83" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M83" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="7"/>
+      <c r="P83" s="7"/>
+      <c r="Q83" s="7"/>
+      <c r="R83" s="7"/>
+      <c r="S83" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T83" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U83" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
         <v>7</v>
       </c>
@@ -3244,17 +3983,25 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
-      <c r="K84" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L84" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M84" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K84" s="7"/>
+      <c r="L84" s="7"/>
+      <c r="M84" s="7"/>
+      <c r="N84" s="7"/>
+      <c r="O84" s="7"/>
+      <c r="P84" s="7"/>
+      <c r="Q84" s="7"/>
+      <c r="R84" s="7"/>
+      <c r="S84" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T84" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U84" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>7</v>
       </c>
@@ -3275,17 +4022,25 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
-      <c r="K85" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L85" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M85" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
+      <c r="Q85" s="7"/>
+      <c r="R85" s="7"/>
+      <c r="S85" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T85" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U85" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>7</v>
       </c>
@@ -3306,17 +4061,25 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
-      <c r="K86" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L86" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M86" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K86" s="7"/>
+      <c r="L86" s="7"/>
+      <c r="M86" s="7"/>
+      <c r="N86" s="7"/>
+      <c r="O86" s="7"/>
+      <c r="P86" s="7"/>
+      <c r="Q86" s="7"/>
+      <c r="R86" s="7"/>
+      <c r="S86" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T86" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U86" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>7</v>
       </c>
@@ -3337,17 +4100,25 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
-      <c r="K87" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L87" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M87" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K87" s="7"/>
+      <c r="L87" s="7"/>
+      <c r="M87" s="7"/>
+      <c r="N87" s="7"/>
+      <c r="O87" s="7"/>
+      <c r="P87" s="7"/>
+      <c r="Q87" s="7"/>
+      <c r="R87" s="7"/>
+      <c r="S87" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T87" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U87" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>7</v>
       </c>
@@ -3368,17 +4139,25 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
-      <c r="K88" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L88" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M88" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K88" s="7"/>
+      <c r="L88" s="7"/>
+      <c r="M88" s="7"/>
+      <c r="N88" s="7"/>
+      <c r="O88" s="7"/>
+      <c r="P88" s="7"/>
+      <c r="Q88" s="7"/>
+      <c r="R88" s="7"/>
+      <c r="S88" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T88" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U88" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>7</v>
       </c>
@@ -3399,17 +4178,25 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-      <c r="K89" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L89" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M89" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K89" s="7"/>
+      <c r="L89" s="7"/>
+      <c r="M89" s="7"/>
+      <c r="N89" s="7"/>
+      <c r="O89" s="7"/>
+      <c r="P89" s="7"/>
+      <c r="Q89" s="7"/>
+      <c r="R89" s="7"/>
+      <c r="S89" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T89" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U89" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>7</v>
       </c>
@@ -3430,17 +4217,25 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
-      <c r="K90" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L90" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M90" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K90" s="7"/>
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+      <c r="N90" s="7"/>
+      <c r="O90" s="7"/>
+      <c r="P90" s="7"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
+      <c r="S90" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T90" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U90" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>7</v>
       </c>
@@ -3461,17 +4256,25 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
-      <c r="K91" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L91" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M91" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="7"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="7"/>
+      <c r="P91" s="7"/>
+      <c r="Q91" s="7"/>
+      <c r="R91" s="7"/>
+      <c r="S91" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T91" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U91" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>7</v>
       </c>
@@ -3492,17 +4295,25 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
-      <c r="K92" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L92" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M92" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K92" s="7"/>
+      <c r="L92" s="7"/>
+      <c r="M92" s="7"/>
+      <c r="N92" s="7"/>
+      <c r="O92" s="7"/>
+      <c r="P92" s="7"/>
+      <c r="Q92" s="7"/>
+      <c r="R92" s="7"/>
+      <c r="S92" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T92" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U92" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>7</v>
       </c>
@@ -3523,17 +4334,25 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
-      <c r="K93" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L93" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M93" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K93" s="7"/>
+      <c r="L93" s="7"/>
+      <c r="M93" s="7"/>
+      <c r="N93" s="7"/>
+      <c r="O93" s="7"/>
+      <c r="P93" s="7"/>
+      <c r="Q93" s="7"/>
+      <c r="R93" s="7"/>
+      <c r="S93" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T93" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U93" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>7</v>
       </c>
@@ -3554,17 +4373,25 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
-      <c r="K94" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L94" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M94" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+      <c r="N94" s="7"/>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
+      <c r="Q94" s="7"/>
+      <c r="R94" s="7"/>
+      <c r="S94" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T94" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U94" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
@@ -3585,17 +4412,25 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
-      <c r="K95" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L95" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M95" s="7">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K95" s="7"/>
+      <c r="L95" s="7"/>
+      <c r="M95" s="7"/>
+      <c r="N95" s="7"/>
+      <c r="O95" s="7"/>
+      <c r="P95" s="7"/>
+      <c r="Q95" s="7"/>
+      <c r="R95" s="7"/>
+      <c r="S95" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T95" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U95" s="7">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>7</v>
       </c>
@@ -3616,17 +4451,26 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
-      <c r="K96" s="7">
-        <v>2001</v>
-      </c>
-      <c r="L96" s="7">
-        <v>2001</v>
-      </c>
-      <c r="M96" s="7">
+      <c r="K96" s="7"/>
+      <c r="L96" s="7"/>
+      <c r="M96" s="7"/>
+      <c r="N96" s="7"/>
+      <c r="O96" s="7"/>
+      <c r="P96" s="7"/>
+      <c r="Q96" s="7"/>
+      <c r="R96" s="7"/>
+      <c r="S96" s="7">
+        <v>2001</v>
+      </c>
+      <c r="T96" s="7">
+        <v>2001</v>
+      </c>
+      <c r="U96" s="7">
         <v>2001</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
removing mention/structure of byproducts
</commit_message>
<xml_diff>
--- a/input_files/user_defined/Scenario setup.xlsx
+++ b/input_files/user_defined/Scenario setup.xlsx
@@ -1,21 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/input_files/user_defined/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jryter_usgs_gov/Documents/Documents/generalizationOutside/generalization/input_files/user_defined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AA0098-7DDC-AA4D-A7F4-A72C07EE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{05AA0098-7DDC-AA4D-A7F4-A72C07EE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{611A0E07-3E32-412B-B53F-4C234CC89A29}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
+    <workbookView xWindow="-6078" yWindow="6384" windowWidth="23232" windowHeight="13992" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1326,14 +1354,14 @@
     <tableColumn id="8" xr3:uid="{BB62F53F-FC7E-0241-8EFE-9D0D4B695FC4}" name="Scenario 3"/>
     <tableColumn id="9" xr3:uid="{71A5D20F-2653-0746-B54E-2208868C584B}" name="Scenario 4"/>
     <tableColumn id="10" xr3:uid="{57545BB2-994C-E14B-995E-1E22F5BA7322}" name="Scenario 5"/>
-    <tableColumn id="22" xr3:uid="{6902B9B4-8E0D-2646-885E-EDD1EE6854F9}" name="Scenario 6" dataDxfId="0"/>
-    <tableColumn id="21" xr3:uid="{0219D9D3-A7AF-B649-9720-C5C56B6DA494}" name="Scenario 7" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{C0DF87A7-EA0E-5549-9DAF-C7D237CAC211}" name="Scenario 8" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{1003B7E9-86E5-BD44-8CF1-08E412F43519}" name="Scenario 9" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{EE68D8F1-C9A3-844D-B61C-BFC4D6C540B4}" name="Scenario 10" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{AF7F194F-8762-1F4B-829B-D2951D37AEDF}" name="Scenario 11" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{CE4B6D99-C26D-3B42-90BF-E046DE5C8035}" name="Scenario 12" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{AB5BD98B-FAF8-304C-9752-E581F8FDFE2E}" name="Scenario 13" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{6902B9B4-8E0D-2646-885E-EDD1EE6854F9}" name="Scenario 6" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{0219D9D3-A7AF-B649-9720-C5C56B6DA494}" name="Scenario 7" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{C0DF87A7-EA0E-5549-9DAF-C7D237CAC211}" name="Scenario 8" dataDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{1003B7E9-86E5-BD44-8CF1-08E412F43519}" name="Scenario 9" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{EE68D8F1-C9A3-844D-B61C-BFC4D6C540B4}" name="Scenario 10" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{AF7F194F-8762-1F4B-829B-D2951D37AEDF}" name="Scenario 11" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{CE4B6D99-C26D-3B42-90BF-E046DE5C8035}" name="Scenario 12" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{AB5BD98B-FAF8-304C-9752-E581F8FDFE2E}" name="Scenario 13" dataDxfId="0"/>
     <tableColumn id="11" xr3:uid="{9EC9A262-BA04-314B-8E87-E93596D98225}" name="Year 1"/>
     <tableColumn id="12" xr3:uid="{3B932622-32D8-EB4D-B8D6-252827BECB68}" name="Year 2"/>
     <tableColumn id="13" xr3:uid="{67C9335A-4404-0B4E-A4E3-F38FEB4535CA}" name="Year 3"/>
@@ -1655,22 +1683,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70A1D66-ACB3-5F43-8146-4761D363CB09}">
   <dimension ref="A1:AI96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="58.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.375" customWidth="1"/>
     <col min="4" max="4" width="89.5" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" style="6" customWidth="1"/>
-    <col min="6" max="18" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.125" style="6" customWidth="1"/>
+    <col min="6" max="18" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1777,7 +1805,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -1794,7 +1822,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1811,7 +1839,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1828,7 +1856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1845,7 +1873,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
@@ -1862,7 +1890,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -1879,7 +1907,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -1896,7 +1924,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -1913,7 +1941,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>116</v>
       </c>
@@ -1930,7 +1958,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -1947,7 +1975,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -1964,7 +1992,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>116</v>
       </c>
@@ -1981,7 +2009,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -1998,7 +2026,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>116</v>
       </c>
@@ -2015,7 +2043,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -2032,7 +2060,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -2049,7 +2077,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -2066,7 +2094,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -2083,7 +2111,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -2100,7 +2128,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>116</v>
       </c>
@@ -2117,7 +2145,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>116</v>
       </c>
@@ -2134,7 +2162,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>116</v>
       </c>
@@ -2151,7 +2179,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>116</v>
       </c>
@@ -2168,7 +2196,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -2185,7 +2213,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -2202,7 +2230,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>116</v>
       </c>
@@ -2219,7 +2247,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>196</v>
       </c>
@@ -2236,7 +2264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -2253,7 +2281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>196</v>
       </c>
@@ -2270,7 +2298,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -2287,7 +2315,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>196</v>
       </c>
@@ -2304,7 +2332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>196</v>
       </c>
@@ -2321,7 +2349,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>196</v>
       </c>
@@ -2338,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>196</v>
       </c>
@@ -2355,7 +2383,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -2372,7 +2400,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>196</v>
       </c>
@@ -2389,7 +2417,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>196</v>
       </c>
@@ -2406,7 +2434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -2423,7 +2451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>196</v>
       </c>
@@ -2440,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -2457,7 +2485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -2474,7 +2502,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -2491,7 +2519,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>196</v>
       </c>
@@ -2508,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>196</v>
       </c>
@@ -2525,7 +2553,7 @@
         <v>20220208</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>196</v>
       </c>
@@ -2542,7 +2570,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>196</v>
       </c>
@@ -2559,7 +2587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>196</v>
       </c>
@@ -2576,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>196</v>
       </c>
@@ -2593,7 +2621,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>254</v>
       </c>
@@ -2670,7 +2698,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>254</v>
       </c>
@@ -2687,7 +2715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -2764,7 +2792,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>254</v>
       </c>
@@ -2838,7 +2866,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>254</v>
       </c>
@@ -2912,7 +2940,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>254</v>
       </c>
@@ -2926,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -2940,7 +2968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>254</v>
       </c>
@@ -2954,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2987,7 +3015,7 @@
       <c r="T58" s="7"/>
       <c r="U58" s="7"/>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>7</v>
       </c>
@@ -3026,7 +3054,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>7</v>
       </c>
@@ -3065,7 +3093,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>7</v>
       </c>
@@ -3104,7 +3132,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>7</v>
       </c>
@@ -3143,7 +3171,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>7</v>
       </c>
@@ -3182,7 +3210,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>7</v>
       </c>
@@ -3221,7 +3249,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>7</v>
       </c>
@@ -3260,7 +3288,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>7</v>
       </c>
@@ -3299,7 +3327,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>7</v>
       </c>
@@ -3338,7 +3366,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>7</v>
       </c>
@@ -3377,7 +3405,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>7</v>
       </c>
@@ -3416,7 +3444,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>7</v>
       </c>
@@ -3455,7 +3483,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>7</v>
       </c>
@@ -3494,7 +3522,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>7</v>
       </c>
@@ -3533,7 +3561,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>7</v>
       </c>
@@ -3572,7 +3600,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>7</v>
       </c>
@@ -3611,7 +3639,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>7</v>
       </c>
@@ -3650,7 +3678,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>7</v>
       </c>
@@ -3689,7 +3717,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>7</v>
       </c>
@@ -3728,7 +3756,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>7</v>
       </c>
@@ -3767,7 +3795,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>7</v>
       </c>
@@ -3806,7 +3834,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>7</v>
       </c>
@@ -3845,7 +3873,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>7</v>
       </c>
@@ -3884,7 +3912,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>7</v>
       </c>
@@ -3923,7 +3951,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>7</v>
       </c>
@@ -3962,7 +3990,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>7</v>
       </c>
@@ -4001,7 +4029,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>7</v>
       </c>
@@ -4040,7 +4068,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>7</v>
       </c>
@@ -4079,7 +4107,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>7</v>
       </c>
@@ -4118,7 +4146,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>7</v>
       </c>
@@ -4157,7 +4185,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>7</v>
       </c>
@@ -4196,7 +4224,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>7</v>
       </c>
@@ -4235,7 +4263,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>7</v>
       </c>
@@ -4274,7 +4302,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>7</v>
       </c>
@@ -4313,7 +4341,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>7</v>
       </c>
@@ -4352,7 +4380,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>7</v>
       </c>
@@ -4391,7 +4419,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>7</v>
       </c>
@@ -4430,7 +4458,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>7</v>
       </c>
@@ -4487,12 +4515,12 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="169.83203125" customWidth="1"/>
+    <col min="1" max="1" width="169.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>299</v>
       </c>
@@ -4500,12 +4528,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>291</v>
       </c>
@@ -4523,7 +4551,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>268</v>
       </c>
@@ -4541,7 +4569,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>269</v>
       </c>
@@ -4559,7 +4587,7 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>271</v>
       </c>
@@ -4577,7 +4605,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>270</v>
       </c>
@@ -4595,7 +4623,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>272</v>
       </c>
@@ -4613,7 +4641,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>311</v>
       </c>
@@ -4631,7 +4659,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>310</v>
       </c>
@@ -4649,7 +4677,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -4665,7 +4693,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>295</v>
       </c>
@@ -4683,7 +4711,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>294</v>
       </c>
@@ -4701,7 +4729,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" ht="88" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>289</v>
       </c>
@@ -4719,7 +4747,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>288</v>
       </c>
@@ -4737,7 +4765,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>297</v>
       </c>
@@ -4755,7 +4783,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -4771,7 +4799,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>296</v>
       </c>
@@ -4789,7 +4817,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" ht="88" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>298</v>
       </c>
@@ -4807,7 +4835,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
-    <row r="20" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -4823,7 +4851,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
-    <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -4839,7 +4867,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
-    <row r="22" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4855,7 +4883,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4871,7 +4899,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4887,7 +4915,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4903,7 +4931,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4919,7 +4947,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
     </row>
-    <row r="27" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>

</xml_diff>

<commit_message>
changing _var suffixes to _std bc accuracy
</commit_message>
<xml_diff>
--- a/input_files/user_defined/Scenario setup.xlsx
+++ b/input_files/user_defined/Scenario setup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/jryter_usgs_gov/Documents/Documents/generalizationOutside/generalization/input_files/user_defined/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{05AA0098-7DDC-AA4D-A7F4-A72C07EE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{611A0E07-3E32-412B-B53F-4C234CC89A29}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{05AA0098-7DDC-AA4D-A7F4-A72C07EE42CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5C23BEA-7DE1-43C3-B738-62339925F4B0}"/>
   <bookViews>
-    <workbookView xWindow="-6078" yWindow="6384" windowWidth="23232" windowHeight="13992" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>Mine size variance</t>
   </si>
   <si>
-    <t>primary_production_var</t>
-  </si>
-  <si>
     <t>The natural log of mine production is normally distributed; this is the standard deviation of that distribution.</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>Mine ore grade variance</t>
   </si>
   <si>
-    <t>primary_ore_grade_var</t>
-  </si>
-  <si>
     <t>Mine fraction, underground</t>
   </si>
   <si>
@@ -1069,6 +1063,12 @@
   </si>
   <si>
     <t>Year 17</t>
+  </si>
+  <si>
+    <t>primary_production_std</t>
+  </si>
+  <si>
+    <t>primary_ore_grade_std</t>
   </si>
 </sst>
 </file>
@@ -1684,8 +1684,8 @@
   <dimension ref="A1:AI96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O55" sqref="O55"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1715,43 +1715,43 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" t="s">
         <v>275</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>276</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>277</v>
       </c>
-      <c r="I1" t="s">
-        <v>278</v>
-      </c>
-      <c r="J1" t="s">
-        <v>279</v>
-      </c>
       <c r="K1" t="s">
+        <v>310</v>
+      </c>
+      <c r="L1" t="s">
         <v>312</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
+        <v>313</v>
+      </c>
+      <c r="N1" t="s">
         <v>314</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>315</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>316</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>317</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>318</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>319</v>
-      </c>
-      <c r="R1" t="s">
-        <v>320</v>
       </c>
       <c r="S1" t="s">
         <v>5</v>
@@ -1760,505 +1760,505 @@
         <v>6</v>
       </c>
       <c r="U1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="V1" t="s">
+        <v>319</v>
+      </c>
+      <c r="W1" t="s">
+        <v>320</v>
+      </c>
+      <c r="X1" t="s">
         <v>321</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>322</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>323</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>324</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>325</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>326</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>327</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>328</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>329</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>330</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>331</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>332</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>333</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="D2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
         <v>121</v>
       </c>
-      <c r="C3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" t="s">
         <v>128</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" s="6" t="s">
         <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" t="s">
         <v>132</v>
       </c>
-      <c r="C7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D7" t="s">
-        <v>134</v>
-      </c>
       <c r="E7" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
         <v>135</v>
       </c>
-      <c r="C8" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" t="s">
-        <v>137</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
         <v>138</v>
       </c>
-      <c r="C9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" t="s">
-        <v>140</v>
-      </c>
       <c r="E9" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
         <v>141</v>
       </c>
-      <c r="C10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" t="s">
-        <v>143</v>
-      </c>
       <c r="E10" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" t="s">
         <v>144</v>
       </c>
-      <c r="C11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" t="s">
-        <v>146</v>
-      </c>
       <c r="E11" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" t="s">
         <v>147</v>
       </c>
-      <c r="C12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D12" t="s">
-        <v>149</v>
-      </c>
       <c r="E12" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
         <v>150</v>
       </c>
-      <c r="C13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" t="s">
-        <v>152</v>
-      </c>
       <c r="E13" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" t="s">
         <v>153</v>
       </c>
-      <c r="C14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" t="s">
-        <v>155</v>
-      </c>
       <c r="E14" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" t="s">
         <v>156</v>
       </c>
-      <c r="C15" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" t="s">
-        <v>158</v>
-      </c>
       <c r="E15" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D16" t="s">
-        <v>309</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D17" t="s">
+        <v>307</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="C17" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" t="s">
-        <v>309</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" t="s">
         <v>162</v>
       </c>
-      <c r="C18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" t="s">
-        <v>164</v>
-      </c>
       <c r="E18" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D19" t="s">
         <v>165</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="D19" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" t="s">
         <v>169</v>
       </c>
-      <c r="C20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D20" t="s">
-        <v>171</v>
-      </c>
       <c r="E20" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" t="s">
         <v>172</v>
       </c>
-      <c r="C21" t="s">
-        <v>173</v>
-      </c>
-      <c r="D21" t="s">
-        <v>174</v>
-      </c>
       <c r="E21" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" t="s">
         <v>175</v>
       </c>
-      <c r="C22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" t="s">
-        <v>177</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23" t="s">
         <v>178</v>
       </c>
-      <c r="C23" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" t="s">
-        <v>180</v>
-      </c>
       <c r="E23" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" t="s">
         <v>181</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="D24" t="s">
-        <v>183</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" t="s">
         <v>185</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="D25" t="s">
-        <v>187</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="s">
         <v>189</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="D26" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" t="s">
         <v>193</v>
       </c>
-      <c r="C27" t="s">
-        <v>194</v>
-      </c>
-      <c r="D27" t="s">
-        <v>195</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C28" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="D28" t="s">
         <v>197</v>
-      </c>
-      <c r="C28" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" t="s">
-        <v>199</v>
       </c>
       <c r="E28" s="6">
         <v>5</v>
@@ -2266,16 +2266,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" t="s">
         <v>200</v>
-      </c>
-      <c r="C29" t="s">
-        <v>201</v>
-      </c>
-      <c r="D29" t="s">
-        <v>202</v>
       </c>
       <c r="E29" s="6">
         <v>3</v>
@@ -2283,33 +2283,33 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C30" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" t="s">
         <v>203</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" s="6" t="s">
         <v>204</v>
-      </c>
-      <c r="D30" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" t="s">
         <v>207</v>
-      </c>
-      <c r="C31" t="s">
-        <v>208</v>
-      </c>
-      <c r="D31" t="s">
-        <v>209</v>
       </c>
       <c r="E31" s="6">
         <v>0.3</v>
@@ -2317,16 +2317,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
         <v>210</v>
-      </c>
-      <c r="C32" t="s">
-        <v>211</v>
-      </c>
-      <c r="D32" t="s">
-        <v>212</v>
       </c>
       <c r="E32" s="6">
         <v>0.5</v>
@@ -2334,16 +2334,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C33" t="s">
+        <v>212</v>
+      </c>
+      <c r="D33" t="s">
         <v>213</v>
-      </c>
-      <c r="C33" t="s">
-        <v>214</v>
-      </c>
-      <c r="D33" t="s">
-        <v>215</v>
       </c>
       <c r="E33" s="6">
         <v>0.2</v>
@@ -2351,16 +2351,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" t="s">
         <v>216</v>
-      </c>
-      <c r="C34" t="s">
-        <v>217</v>
-      </c>
-      <c r="D34" t="s">
-        <v>218</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
@@ -2368,16 +2368,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" t="s">
         <v>219</v>
-      </c>
-      <c r="C35" t="s">
-        <v>220</v>
-      </c>
-      <c r="D35" t="s">
-        <v>221</v>
       </c>
       <c r="E35" s="6">
         <v>0.4</v>
@@ -2385,16 +2385,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" t="s">
+        <v>218</v>
+      </c>
+      <c r="D36" t="s">
         <v>219</v>
-      </c>
-      <c r="C36" t="s">
-        <v>220</v>
-      </c>
-      <c r="D36" t="s">
-        <v>221</v>
       </c>
       <c r="E36" s="6">
         <v>0.4</v>
@@ -2402,16 +2402,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" t="s">
         <v>222</v>
-      </c>
-      <c r="C37" t="s">
-        <v>223</v>
-      </c>
-      <c r="D37" t="s">
-        <v>224</v>
       </c>
       <c r="E37" s="6">
         <v>0.4</v>
@@ -2419,16 +2419,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" t="s">
         <v>225</v>
-      </c>
-      <c r="C38" t="s">
-        <v>226</v>
-      </c>
-      <c r="D38" t="s">
-        <v>227</v>
       </c>
       <c r="E38" s="6">
         <v>3</v>
@@ -2436,16 +2436,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" t="s">
         <v>225</v>
-      </c>
-      <c r="C39" t="s">
-        <v>226</v>
-      </c>
-      <c r="D39" t="s">
-        <v>227</v>
       </c>
       <c r="E39" s="6">
         <v>3</v>
@@ -2453,16 +2453,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C40" t="s">
+        <v>227</v>
+      </c>
+      <c r="D40" t="s">
         <v>228</v>
-      </c>
-      <c r="C40" t="s">
-        <v>229</v>
-      </c>
-      <c r="D40" t="s">
-        <v>230</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
@@ -2470,16 +2470,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C41" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" t="s">
         <v>231</v>
-      </c>
-      <c r="C41" t="s">
-        <v>232</v>
-      </c>
-      <c r="D41" t="s">
-        <v>233</v>
       </c>
       <c r="E41" s="6">
         <v>10</v>
@@ -2487,16 +2487,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" t="s">
         <v>234</v>
-      </c>
-      <c r="C42" t="s">
-        <v>235</v>
-      </c>
-      <c r="D42" t="s">
-        <v>236</v>
       </c>
       <c r="E42" s="6">
         <v>10</v>
@@ -2504,16 +2504,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C43" t="s">
+        <v>236</v>
+      </c>
+      <c r="D43" t="s">
         <v>237</v>
-      </c>
-      <c r="C43" t="s">
-        <v>238</v>
-      </c>
-      <c r="D43" t="s">
-        <v>239</v>
       </c>
       <c r="E43" s="6">
         <v>0.1</v>
@@ -2521,16 +2521,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C44" t="s">
+        <v>243</v>
+      </c>
+      <c r="D44" t="s">
         <v>244</v>
-      </c>
-      <c r="C44" t="s">
-        <v>245</v>
-      </c>
-      <c r="D44" t="s">
-        <v>246</v>
       </c>
       <c r="E44" s="6">
         <v>1</v>
@@ -2538,16 +2538,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C45" t="s">
+        <v>246</v>
+      </c>
+      <c r="D45" t="s">
         <v>247</v>
-      </c>
-      <c r="C45" t="s">
-        <v>248</v>
-      </c>
-      <c r="D45" t="s">
-        <v>249</v>
       </c>
       <c r="E45" s="6">
         <v>20220208</v>
@@ -2555,16 +2555,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C46" t="s">
+        <v>249</v>
+      </c>
+      <c r="D46" t="s">
         <v>250</v>
-      </c>
-      <c r="C46" t="s">
-        <v>251</v>
-      </c>
-      <c r="D46" t="s">
-        <v>252</v>
       </c>
       <c r="E46" s="6">
         <v>0.95</v>
@@ -2572,16 +2572,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C47" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D47" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E47" s="6">
         <v>20</v>
@@ -2589,16 +2589,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C48" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E48" s="6" t="b">
         <v>1</v>
@@ -2606,33 +2606,33 @@
     </row>
     <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C49" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D49" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C50" t="s">
+        <v>239</v>
+      </c>
+      <c r="D50" t="s">
         <v>240</v>
-      </c>
-      <c r="C50" t="s">
-        <v>241</v>
-      </c>
-      <c r="D50" t="s">
-        <v>242</v>
       </c>
       <c r="E50" s="6" t="b">
         <v>1</v>
@@ -2700,16 +2700,16 @@
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C51" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D51" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E51" s="6" t="b">
         <v>1</v>
@@ -2717,16 +2717,16 @@
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C52" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D52" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E52" s="6">
         <v>1</v>
@@ -2794,16 +2794,16 @@
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>252</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" t="s">
         <v>254</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C53" t="s">
-        <v>256</v>
-      </c>
       <c r="D53" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E53" s="6">
         <v>0</v>
@@ -2868,16 +2868,16 @@
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C54" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D54" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E54" s="6">
         <v>0</v>
@@ -2942,13 +2942,13 @@
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C55" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E55" s="6">
         <v>1</v>
@@ -2956,13 +2956,13 @@
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C56" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E56" s="6">
         <v>0</v>
@@ -2970,13 +2970,13 @@
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C57" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E57" s="6">
         <v>0</v>
@@ -2993,7 +2993,7 @@
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E58" s="6">
         <v>2.546855E-2</v>
@@ -3029,7 +3029,7 @@
         <v>12</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
@@ -3068,7 +3068,7 @@
         <v>15</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
@@ -3107,7 +3107,7 @@
         <v>18</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
@@ -3146,7 +3146,7 @@
         <v>21</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -3185,7 +3185,7 @@
         <v>24</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -3224,7 +3224,7 @@
         <v>27</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -3263,7 +3263,7 @@
         <v>30</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -3302,7 +3302,7 @@
         <v>33</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -3341,7 +3341,7 @@
         <v>36</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -3380,7 +3380,7 @@
         <v>39</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -3419,7 +3419,7 @@
         <v>42</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -3458,7 +3458,7 @@
         <v>45</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -3497,7 +3497,7 @@
         <v>48</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -3536,7 +3536,7 @@
         <v>51</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
@@ -3575,7 +3575,7 @@
         <v>54</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
@@ -3614,7 +3614,7 @@
         <v>57</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -3650,10 +3650,10 @@
         <v>59</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -3689,10 +3689,10 @@
         <v>61</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -3728,10 +3728,10 @@
         <v>63</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -3767,10 +3767,10 @@
         <v>65</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -3806,10 +3806,10 @@
         <v>67</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -3848,7 +3848,7 @@
         <v>70</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -3887,7 +3887,7 @@
         <v>73</v>
       </c>
       <c r="E81" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -3926,7 +3926,7 @@
         <v>76</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -3965,7 +3965,7 @@
         <v>79</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -4004,7 +4004,7 @@
         <v>82</v>
       </c>
       <c r="E84" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -4043,7 +4043,7 @@
         <v>84</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -4082,7 +4082,7 @@
         <v>86</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
@@ -4121,7 +4121,7 @@
         <v>89</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
@@ -4154,13 +4154,13 @@
         <v>90</v>
       </c>
       <c r="C88" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D88" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="E88" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -4190,16 +4190,16 @@
         <v>7</v>
       </c>
       <c r="B89" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="D89" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D89" s="7" t="s">
-        <v>95</v>
-      </c>
       <c r="E89" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
@@ -4229,16 +4229,16 @@
         <v>7</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>97</v>
+        <v>334</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -4268,16 +4268,16 @@
         <v>7</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C91" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>100</v>
-      </c>
       <c r="E91" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -4307,16 +4307,16 @@
         <v>7</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C92" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="E92" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
@@ -4346,16 +4346,16 @@
         <v>7</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C93" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="E93" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
@@ -4385,16 +4385,16 @@
         <v>7</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C94" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="E94" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
@@ -4424,16 +4424,16 @@
         <v>7</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C95" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="E95" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
@@ -4463,16 +4463,16 @@
         <v>7</v>
       </c>
       <c r="B96" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D96" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C96" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="E96" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
@@ -4522,20 +4522,20 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4553,7 +4553,7 @@
     </row>
     <row r="4" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="5" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -4589,7 +4589,7 @@
     </row>
     <row r="6" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="7" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="8" spans="1:14" ht="42" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="9" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="12" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="13" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="14" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4749,7 +4749,7 @@
     </row>
     <row r="15" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="16" spans="1:14" ht="126" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="18" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="19" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>

</xml_diff>